<commit_message>
Second Order Stations update
QC for 1893 and 1894 complete
</commit_message>
<xml_diff>
--- a/second-order/1894/February1894.xlsx
+++ b/second-order/1894/February1894.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27916"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metoffice-my.sharepoint.com/personal/catherine_ross_metoffice_gov_uk/Documents/2nd Order Stations/1894/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11904" documentId="13_ncr:1_{54B9FF61-BCA2-4E60-9BB7-8B5FD9CFC0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21164037-2EFF-44A7-A9D1-0C049F378C66}"/>
+  <xr:revisionPtr revIDLastSave="12662" documentId="13_ncr:1_{54B9FF61-BCA2-4E60-9BB7-8B5FD9CFC0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C98435A-E1D1-4665-93AF-CC2CF5C5EA74}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="832" firstSheet="20" activeTab="20" xr2:uid="{F301734F-2AF4-4BAC-817B-B629B6303572}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="832" firstSheet="5" activeTab="20" xr2:uid="{F301734F-2AF4-4BAC-817B-B629B6303572}"/>
   </bookViews>
   <sheets>
     <sheet name="Deerness" sheetId="15" r:id="rId1"/>
@@ -48,6 +48,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -883,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4108655-B436-409A-BEA1-C15E2C901F28}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
@@ -2396,7 +2397,7 @@
         <v>39.799999999999997</v>
       </c>
       <c r="I24" s="1">
-        <v>35.799999999999997</v>
+        <v>35</v>
       </c>
       <c r="J24" s="6">
         <v>44.6</v>
@@ -2964,7 +2965,7 @@
         <v>37</v>
       </c>
       <c r="I32" s="1">
-        <v>54.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="J32" s="6">
         <v>40</v>
@@ -3094,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F58535-F46B-4397-857F-B5B0AFE46BF9}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView topLeftCell="U21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4365,7 +4366,7 @@
         <v>10</v>
       </c>
       <c r="W20" s="9">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1">
@@ -5302,10 +5303,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2D65C3-F0FC-43D4-8EDF-7503FE5358F7}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:T2"/>
+    <sheetView topLeftCell="P21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -6953,7 +6954,7 @@
         <v>30.11</v>
       </c>
       <c r="G26" s="1">
-        <v>287</v>
+        <v>28.7</v>
       </c>
       <c r="H26" s="1">
         <v>26.8</v>
@@ -7493,6 +7494,12 @@
       </c>
       <c r="W33" s="13">
         <v>1.34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>29.870357142857149</v>
       </c>
     </row>
   </sheetData>
@@ -7514,8 +7521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD0F272-B8A4-46FC-A472-771D73413392}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView topLeftCell="M31" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7669,7 +7676,7 @@
         <v>29.23</v>
       </c>
       <c r="F5" s="6">
-        <v>29.48</v>
+        <v>29.13</v>
       </c>
       <c r="G5" s="1">
         <v>35.200000000000003</v>
@@ -9722,10 +9729,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD84A6CC-49D4-47FD-9DBF-F07FCE349F1A}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView topLeftCell="K20" workbookViewId="0">
+      <selection activeCell="AC34" sqref="AC34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -11913,6 +11920,12 @@
       </c>
       <c r="W33" s="13">
         <v>2.1120000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>29.779642857142857</v>
       </c>
     </row>
   </sheetData>
@@ -11932,9 +11945,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F522100-1AF0-43D4-A080-F24B7139868C}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="O21" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
@@ -13364,10 +13377,10 @@
         <v>19</v>
       </c>
       <c r="E23" s="5">
-        <v>29.47</v>
+        <v>30.47</v>
       </c>
       <c r="F23" s="6">
-        <v>29.41</v>
+        <v>30.41</v>
       </c>
       <c r="G23" s="1">
         <v>32.1</v>
@@ -13435,10 +13448,10 @@
         <v>20</v>
       </c>
       <c r="E24" s="5">
-        <v>29.38</v>
+        <v>30.38</v>
       </c>
       <c r="F24" s="6">
-        <v>29.31</v>
+        <v>30.31</v>
       </c>
       <c r="G24" s="1">
         <v>33.5</v>
@@ -13506,10 +13519,10 @@
         <v>21</v>
       </c>
       <c r="E25" s="5">
-        <v>29.23</v>
+        <v>30.23</v>
       </c>
       <c r="F25" s="6">
-        <v>29.21</v>
+        <v>30.21</v>
       </c>
       <c r="G25" s="1">
         <v>35.6</v>
@@ -14123,6 +14136,12 @@
       </c>
       <c r="W33" s="13">
         <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.969642857142862</v>
       </c>
     </row>
   </sheetData>
@@ -14142,10 +14161,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42ABBC7C-B157-4A4E-8414-C98E473BD393}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView topLeftCell="Q21" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -14391,7 +14410,7 @@
         <v>1.6</v>
       </c>
       <c r="M6" s="5">
-        <v>0.312</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="N6" s="6">
         <v>0.314</v>
@@ -14441,7 +14460,7 @@
         <v>29.98</v>
       </c>
       <c r="F7" s="6">
-        <v>29.35</v>
+        <v>30.35</v>
       </c>
       <c r="G7" s="1">
         <v>47.3</v>
@@ -16333,6 +16352,12 @@
       </c>
       <c r="W33" s="13">
         <v>2.234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>30.000357142857137</v>
       </c>
     </row>
   </sheetData>
@@ -16352,15 +16377,16 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D9C1B2-8C1C-4225-9D26-AF6DAC2640AF}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" workbookViewId="0">
+    <sheetView topLeftCell="M21" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" s="2" customFormat="1" ht="29.1">
@@ -16604,7 +16630,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="N6" s="6">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="O6" s="1">
         <v>91</v>
@@ -17734,7 +17760,7 @@
         <v>1.3</v>
       </c>
       <c r="L22" s="6">
-        <v>0.28999999999999998</v>
+        <v>2.9</v>
       </c>
       <c r="M22" s="5">
         <v>0.219</v>
@@ -18543,6 +18569,16 @@
       </c>
       <c r="W33" s="13">
         <v>2.621</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.91892857142857</v>
+      </c>
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>29.916428571428565</v>
       </c>
     </row>
   </sheetData>
@@ -18562,10 +18598,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B53C70-E59B-4757-99CF-9D169C92385B}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="R21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -20423,7 +20459,7 @@
         <v>29.06</v>
       </c>
       <c r="F29" s="6">
-        <v>20.16</v>
+        <v>29.16</v>
       </c>
       <c r="G29" s="1">
         <v>49.7</v>
@@ -20743,7 +20779,7 @@
         <v>31</v>
       </c>
       <c r="T33" s="12">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="U33" s="10">
         <v>8.3000000000000007</v>
@@ -20753,6 +20789,16 @@
       </c>
       <c r="W33" s="13">
         <v>5.93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.699999999999996</v>
+      </c>
+      <c r="N34">
+        <f>SUM(N5:N32)/28</f>
+        <v>0.23839285714285716</v>
       </c>
     </row>
   </sheetData>
@@ -20772,10 +20818,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5AAE48-C411-4E25-8B1D-2232EA02C65B}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView topLeftCell="L21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -22963,6 +23009,16 @@
       </c>
       <c r="W33" s="13">
         <v>3.6120000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.612857142857141</v>
+      </c>
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>29.60464285714286</v>
       </c>
     </row>
   </sheetData>
@@ -22984,8 +23040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E413A142-C323-471B-8DE8-71C83ABC936E}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView topLeftCell="M22" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -25194,8 +25250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB82F61C-05AA-4FA3-BD74-74225C388CDC}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="L21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -26414,7 +26470,7 @@
         <v>29.94</v>
       </c>
       <c r="F20" s="6">
-        <v>29.08</v>
+        <v>30.08</v>
       </c>
       <c r="G20" s="1">
         <v>39.4</v>
@@ -27402,9 +27458,9 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBA7423-C2C7-4634-AC7C-BDA41601DD7D}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="S21" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
@@ -29593,6 +29649,12 @@
       </c>
       <c r="W33" s="13">
         <v>2.35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>29.727857142857143</v>
       </c>
     </row>
   </sheetData>
@@ -29614,8 +29676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0278F3C-D8F2-4AEA-9D02-7DEF220B388F}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView tabSelected="1" topLeftCell="L29" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -30074,7 +30136,7 @@
         <v>0.9</v>
       </c>
       <c r="M9" s="5">
-        <v>0.247</v>
+        <v>0.23</v>
       </c>
       <c r="N9" s="6">
         <v>0.247</v>
@@ -31823,11 +31885,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CBB8FD-655A-4863-88F4-7CCF8E717079}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:X34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="B30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="3" topLeftCell="S25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X34" sqref="X34"/>
       <selection activeCell="B5" sqref="B5:B32"/>
     </sheetView>
   </sheetViews>
@@ -32039,7 +32101,7 @@
         <v>7</v>
       </c>
       <c r="W5" s="9">
-        <v>0.27600000000000002</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -33127,7 +33189,7 @@
         <v>28.99</v>
       </c>
       <c r="G21" s="1">
-        <v>3.6</v>
+        <v>33.6</v>
       </c>
       <c r="H21" s="1">
         <v>33.9</v>
@@ -33959,7 +34021,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:24">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -34023,6 +34085,26 @@
       <c r="W33" s="13">
         <v>5.68</v>
       </c>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="R34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -34043,9 +34125,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85204B69-BD73-463D-846C-48564885D419}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="O21" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
@@ -35017,7 +35099,7 @@
         <v>48</v>
       </c>
       <c r="R16" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>48</v>
@@ -35644,7 +35726,7 @@
         <v>0.214</v>
       </c>
       <c r="N25" s="6">
-        <v>0.108</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="O25" s="1">
         <v>83</v>
@@ -36234,6 +36316,12 @@
       </c>
       <c r="W33" s="13">
         <v>9.81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="F34">
+        <f>SUM(F5:F32)/28</f>
+        <v>29.653928571428573</v>
       </c>
     </row>
   </sheetData>
@@ -36253,9 +36341,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8320C5D-44A6-4787-84A6-B2499FADF3C6}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="O21" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
@@ -37363,7 +37451,7 @@
         <v>81</v>
       </c>
       <c r="P18" s="6">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>34</v>
@@ -38444,6 +38532,12 @@
       </c>
       <c r="W33" s="13">
         <v>4.47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.548928571428579</v>
       </c>
     </row>
   </sheetData>
@@ -38463,10 +38557,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D07B89-795F-47D1-B9D9-3952301305F5}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+    <sheetView topLeftCell="P21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -39848,7 +39942,7 @@
         <v>3.1</v>
       </c>
       <c r="M22" s="5">
-        <v>0.14699999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="N22" s="6">
         <v>0.14699999999999999</v>
@@ -40654,6 +40748,12 @@
       </c>
       <c r="W33" s="13">
         <v>9.1809999999999992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.563928571428573</v>
       </c>
     </row>
   </sheetData>
@@ -40675,8 +40775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3123BD-0C11-44C5-98B9-64CC39BFEE8C}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="Q25" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -42885,7 +42985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2E6BE9-1CB1-46BB-B103-F378C28219E9}">
   <dimension ref="A2:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="B27" workbookViewId="0">
+    <sheetView topLeftCell="N25" workbookViewId="0">
       <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
@@ -45093,10 +45193,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0FE9D5-A80F-41C9-AEC8-6E2C403BE377}">
-  <dimension ref="A2:W33"/>
+  <dimension ref="A2:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="M21" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -47284,6 +47384,12 @@
       </c>
       <c r="W33" s="13">
         <v>5.6260000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="E34">
+        <f>SUM(E5:E32)/28</f>
+        <v>29.729642857142856</v>
       </c>
     </row>
   </sheetData>
@@ -47302,28 +47408,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Preview xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Preview>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xsi:nil="true"/>
-    <_dlc_DocId xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">H7Q62YT2XCZT-908671883-39968</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">
-      <Url>https://metoffice.sharepoint.com/sites/metofficelibraryarchiveteam/_layouts/15/DocIdRedir.aspx?ID=H7Q62YT2XCZT-908671883-39968</Url>
-      <Description>H7Q62YT2XCZT-908671883-39968</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100005F0ACF65EC5C4F8622AE277C35A390" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a11f18feb37c278a512788b2e5a06b2f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xmlns:ns3="502a79df-4f52-4757-ac2f-753e065f4c93" xmlns:ns4="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d97308c79b2bb5835a55e257627f43a5" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100005F0ACF65EC5C4F8622AE277C35A390" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a4f56144ecba6ff6a413504c0ec2b8c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xmlns:ns3="502a79df-4f52-4757-ac2f-753e065f4c93" xmlns:ns4="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dcae21ac380e060fa17aa32c946feec" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="09baef80-0d7a-4cab-b988-bb3d9fc0663b"/>
     <xsd:import namespace="502a79df-4f52-4757-ac2f-753e065f4c93"/>
@@ -47355,6 +47500,8 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -47453,6 +47600,16 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="29" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="30" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="31" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -47622,77 +47779,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Preview xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Preview>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xsi:nil="true"/>
+    <_dlc_DocId xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">H7Q62YT2XCZT-908671883-39968</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">
+      <Url>https://metoffice.sharepoint.com/sites/metofficelibraryarchiveteam/_layouts/15/DocIdRedir.aspx?ID=H7Q62YT2XCZT-908671883-39968</Url>
+      <Description>H7Q62YT2XCZT-908671883-39968</Description>
+    </_dlc_DocIdUrl>
+    <TaxCatchAll xmlns="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37504570-BFED-402B-9995-BC94451CA335}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{809FA531-E640-4694-8F3D-B3433DDE3267}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D75A9210-C1BB-47FB-9B6D-F3D6FAB58718}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9505B43A-A7A6-4906-BA4A-6D6065F35B07}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9505B43A-A7A6-4906-BA4A-6D6065F35B07}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF423A26-BAAC-41FD-B61D-B32E9031CA3E}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{809FA531-E640-4694-8F3D-B3433DDE3267}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37504570-BFED-402B-9995-BC94451CA335}"/>
 </file>
</xml_diff>